<commit_message>
Update for week 3 turn in
week 3 tunin
organization
replacing SRS 830 on main page
</commit_message>
<xml_diff>
--- a/Time Tracking/CEIS400- WEEK 3 Anaum Syed Time Sheet (2).xlsx
+++ b/Time Tracking/CEIS400- WEEK 3 Anaum Syed Time Sheet (2).xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/15b881ec34b0dbf0/Desktop/CEIS400/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7d037e0306ecfb5d/Desktop/repos_cloned_here_laptop/silver-goggles/Time Tracking/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="8_{7AB79022-6795-43C2-B617-028B8B0767FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2820" yWindow="612" windowWidth="18696" windowHeight="12912" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Member One" sheetId="1" r:id="rId1"/>
@@ -1075,7 +1075,7 @@
   <dimension ref="A1:E48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>

</xml_diff>